<commit_message>
Some CSVs had invalid accounting Years. Rectified them in live spreadsheets.
</commit_message>
<xml_diff>
--- a/csv/main-files/Sahkarnagar.xlsx
+++ b/csv/main-files/Sahkarnagar.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="135">
   <si>
     <t>Prabhag 57A : Smita Vaste</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Benches</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>Pavement blocks</t>
   </si>
   <si>
@@ -84,9 +87,6 @@
   </si>
   <si>
     <t>72/77</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>Toilet- building / Renovation/Maintenance</t>
@@ -143,34 +143,19 @@
     <t>123/127</t>
   </si>
   <si>
-    <t>2016 - 2016</t>
-  </si>
-  <si>
     <t>Installation direction boards</t>
-  </si>
-  <si>
-    <t>2017 - 2016</t>
   </si>
   <si>
     <t xml:space="preserve"> Toilet- building </t>
   </si>
   <si>
-    <t>2018 - 2016</t>
-  </si>
-  <si>
     <t>Toilet Renovation</t>
-  </si>
-  <si>
-    <t>2019 - 2016</t>
   </si>
   <si>
     <t>Fencing, walls</t>
   </si>
   <si>
     <t>FE</t>
-  </si>
-  <si>
-    <t>2020 - 2016</t>
   </si>
   <si>
     <r>
@@ -182,15 +167,6 @@
     <r>
       <t xml:space="preserve">uilding shed </t>
     </r>
-  </si>
-  <si>
-    <t>2021 - 2016</t>
-  </si>
-  <si>
-    <t>2022 - 2016</t>
-  </si>
-  <si>
-    <t>2023 - 2016</t>
   </si>
   <si>
     <t>Develpoment Work</t>
@@ -620,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -730,9 +706,6 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -918,7 +891,7 @@
         <v>150251.0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -931,13 +904,13 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="12">
         <v>107726.0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -950,13 +923,13 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="20">
         <v>192175.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -969,13 +942,13 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="20">
         <v>192850.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -988,13 +961,13 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="20">
         <v>78029.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -1003,7 +976,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="24" t="str">
         <f>SUM(D3:D7)</f>
@@ -1015,30 +988,30 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10">
         <v>1.0</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="12">
         <v>141654.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="14">
         <v>0.0</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10">
         <v>2.0</v>
@@ -1050,33 +1023,33 @@
         <v>162558.0</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10">
         <v>3.0</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="12">
         <v>158597.0</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>4.0</v>
@@ -1095,7 +1068,7 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>5.0</v>
@@ -1114,7 +1087,7 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>6.0</v>
@@ -1133,7 +1106,7 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>7.0</v>
@@ -1152,7 +1125,7 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>8.0</v>
@@ -1173,7 +1146,7 @@
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="24" t="str">
         <f>SUM(D11:D18)</f>
@@ -1305,7 +1278,7 @@
       <c r="A26" s="21"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D26" s="24" t="str">
         <f>SUM(D20:D25)</f>
@@ -1340,32 +1313,32 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B28" s="10">
         <v>2.0</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="12">
         <v>146993.0</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B29" s="10">
         <v>3.0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" s="12">
         <v>169303.0</v>
@@ -1378,13 +1351,13 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B30" s="10">
         <v>4.0</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="12">
         <v>40380.0</v>
@@ -1397,32 +1370,32 @@
     </row>
     <row r="31">
       <c r="A31" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B31" s="10">
         <v>5.0</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D31" s="12">
         <v>87365.0</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B32" s="10">
         <v>6.0</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D32" s="12">
         <v>169820.0</v>
@@ -1435,7 +1408,7 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B33" s="10">
         <v>7.0</v>
@@ -1454,32 +1427,32 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B34" s="10">
         <v>8.0</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="12">
         <v>91122.0</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B35" s="10">
         <v>9.0</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D35" s="12">
         <v>62704.0</v>
@@ -1494,7 +1467,7 @@
       <c r="A36" s="21"/>
       <c r="B36" s="22"/>
       <c r="C36" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D36" s="24" t="str">
         <f>SUM(D27:D35)</f>
@@ -1515,7 +1488,7 @@
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D38" s="34" t="str">
         <f>(D10+D19+D26+D36)</f>
@@ -8370,7 +8343,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -8410,13 +8383,13 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D3" s="12">
         <v>200000.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F3" s="14">
         <v>0.0</v>
@@ -8433,7 +8406,7 @@
         <v>2.0</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D4" s="12">
         <v>104339.0</v>
@@ -8477,7 +8450,7 @@
         <v>124644.0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -8490,13 +8463,13 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="20">
         <v>193586.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -8505,7 +8478,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="24" t="str">
         <f>SUM(D3:D7)</f>
@@ -8517,7 +8490,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10">
         <v>1.0</v>
@@ -8535,37 +8508,37 @@
         <v>0.0</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="10">
         <v>2.0</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D10" s="12">
         <v>121092.0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10">
         <v>3.0</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D11" s="12">
         <v>134103.0</v>
@@ -8578,7 +8551,7 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10">
         <v>4.0</v>
@@ -8597,70 +8570,70 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10">
         <v>5.0</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D13" s="12">
         <v>160225.0</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>6.0</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D14" s="12">
         <v>158682.0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>7.0</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D15" s="12">
         <v>74731.0</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>8.0</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D16" s="12">
         <v>165339.0</v>
@@ -8673,19 +8646,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>9.0</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D17" s="12">
         <v>134286.0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -8694,7 +8667,7 @@
       <c r="A18" s="21"/>
       <c r="B18" s="22"/>
       <c r="C18" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="24" t="str">
         <f>SUM(D9:D17)</f>
@@ -8712,7 +8685,7 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D19" s="12">
         <v>154158.0</v>
@@ -8735,7 +8708,7 @@
         <v>2.0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D20" s="12">
         <v>99278.0</v>
@@ -8754,7 +8727,7 @@
         <v>3.0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D21" s="12">
         <v>118857.0</v>
@@ -8773,13 +8746,13 @@
         <v>4.0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D22" s="12">
         <v>156420.0</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -8792,7 +8765,7 @@
         <v>5.0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D23" s="12">
         <v>91777.0</v>
@@ -8830,7 +8803,7 @@
         <v>7.0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D25" s="12">
         <v>99173.0</v>
@@ -8849,7 +8822,7 @@
         <v>8.0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D26" s="12">
         <v>78708.0</v>
@@ -8864,7 +8837,7 @@
       <c r="A27" s="21"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="24" t="str">
         <f>SUM(D19:D26)</f>
@@ -8882,7 +8855,7 @@
         <v>1.0</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D28" s="12">
         <v>126967.0</v>
@@ -8894,7 +8867,7 @@
         <v>0.0</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29">
@@ -8924,13 +8897,13 @@
         <v>3.0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D30" s="12">
         <v>125675.0</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -8952,7 +8925,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="22"/>
       <c r="C32" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="24" t="str">
         <f>SUM(D28:D31)</f>
@@ -8973,7 +8946,7 @@
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D34" s="34" t="str">
         <f>(D8+D18+D27+D32)</f>
@@ -11947,7 +11920,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -11996,13 +11969,13 @@
         <v>120821.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" s="14">
         <v>0.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H3" s="14">
         <v>87.87</v>
@@ -12022,7 +11995,7 @@
         <v>120821.0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -12042,7 +12015,7 @@
         <v>158573.0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -12056,13 +12029,13 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="12">
         <v>194069.0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -12076,13 +12049,13 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="12">
         <v>185732.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -12092,7 +12065,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="24" t="str">
         <f>SUM(D3:D7)</f>
@@ -12105,7 +12078,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10">
         <v>1.0</v>
@@ -12117,13 +12090,13 @@
         <v>145168.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F9" s="14">
         <v>0.0</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H9" s="14">
         <v>89.0</v>
@@ -12131,19 +12104,19 @@
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="10">
         <v>2.0</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D10" s="12">
         <v>80228.0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -12151,7 +12124,7 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10">
         <v>3.0</v>
@@ -12163,7 +12136,7 @@
         <v>134855.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -12171,13 +12144,13 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10">
         <v>4.0</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D12" s="12">
         <v>136085.0</v>
@@ -12191,19 +12164,19 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10">
         <v>5.0</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="12">
         <v>158280.0</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -12211,19 +12184,19 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>6.0</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="12">
         <v>154287.0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -12231,7 +12204,7 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>7.0</v>
@@ -12243,7 +12216,7 @@
         <v>140490.0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -12251,19 +12224,19 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>8.0</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D16" s="12">
         <v>97390.0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -12271,19 +12244,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>9.0</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" s="12">
         <v>110441.0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -12293,7 +12266,7 @@
       <c r="A18" s="21"/>
       <c r="B18" s="22"/>
       <c r="C18" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="24" t="str">
         <f>SUM(D9:D17)</f>
@@ -12312,22 +12285,22 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D19" s="12">
         <v>139388.0</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F19" s="14">
         <v>1.0</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
@@ -12344,7 +12317,7 @@
         <v>131436.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -12364,7 +12337,7 @@
         <v>131436.0</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -12378,13 +12351,13 @@
         <v>4.0</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D22" s="12">
         <v>148000.0</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -12398,7 +12371,7 @@
         <v>5.0</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D23" s="20">
         <v>77990.0</v>
@@ -12418,13 +12391,13 @@
         <v>6.0</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D24" s="20">
         <v>154996.0</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -12438,13 +12411,13 @@
         <v>7.0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D25" s="20">
         <v>37644.0</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
@@ -12458,13 +12431,13 @@
         <v>8.0</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" s="20">
         <v>133400.0</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -12528,7 +12501,7 @@
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
       <c r="C30" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D30" s="24" t="str">
         <f>SUM(D19:D29)</f>
@@ -12547,7 +12520,7 @@
         <v>1.0</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D31" s="12">
         <v>84791.0</v>
@@ -12559,21 +12532,21 @@
         <v>0.0</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" s="10">
         <v>2.0</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D32" s="12">
         <v>135340.0</v>
@@ -12587,7 +12560,7 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B33" s="10">
         <v>3.0</v>
@@ -12599,7 +12572,7 @@
         <v>134482.0</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -12607,7 +12580,7 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B34" s="10">
         <v>4.0</v>
@@ -12618,8 +12591,8 @@
       <c r="D34" s="12">
         <v>134482.0</v>
       </c>
-      <c r="E34" s="39" t="s">
-        <v>22</v>
+      <c r="E34" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -12627,19 +12600,19 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B35" s="10">
         <v>5.0</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D35" s="12">
         <v>126430.0</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -12647,13 +12620,13 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B36" s="10">
         <v>6.0</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D36" s="12">
         <v>135340.0</v>
@@ -12667,19 +12640,19 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B37" s="10">
         <v>7.0</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D37" s="12">
         <v>114912.0</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -12687,19 +12660,19 @@
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B38" s="10">
         <v>8.0</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D38" s="12">
         <v>67489.0</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -12707,7 +12680,7 @@
     </row>
     <row r="39">
       <c r="A39" s="9" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B39" s="10">
         <v>9.0</v>
@@ -12729,7 +12702,7 @@
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" s="24" t="str">
         <f>SUM(D31:D39)</f>
@@ -12751,7 +12724,7 @@
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D42" s="34" t="str">
         <f>(D8+D18+D30+D40)</f>
@@ -15730,7 +15703,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -15762,7 +15735,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
@@ -15779,13 +15752,13 @@
         <v>122726.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" s="14">
         <v>0.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H3" s="14">
         <v>68.0</v>
@@ -15825,7 +15798,7 @@
         <v>40908.0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -15839,7 +15812,7 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D6" s="12">
         <v>100440.0</v>
@@ -15859,13 +15832,13 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="12">
         <v>192218.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -15879,13 +15852,13 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="12">
         <v>192141.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -15899,13 +15872,13 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="12">
         <v>193348.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -15915,7 +15888,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="24" t="str">
         <f>SUM(D3:D9)</f>
@@ -15928,7 +15901,7 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10">
         <v>1.0</v>
@@ -15940,13 +15913,13 @@
         <v>117788.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F11" s="14">
         <v>0.0</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H11" s="14">
         <v>49.0</v>
@@ -15954,7 +15927,7 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10">
         <v>2.0</v>
@@ -15966,7 +15939,7 @@
         <v>117910.0</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -15974,18 +15947,18 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10">
         <v>3.0</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D13" s="12">
         <v>167842.0</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="16"/>
@@ -15994,7 +15967,7 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>4.0</v>
@@ -16006,7 +15979,7 @@
         <v>150996.0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -16014,13 +15987,13 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>5.0</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="12">
         <v>144301.0</v>
@@ -16034,19 +16007,19 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>6.0</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D16" s="12">
         <v>140443.0</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>96</v>
+      <c r="E16" s="39" t="s">
+        <v>88</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -16054,19 +16027,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>7.0</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D17" s="12">
         <v>140042.0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -16074,19 +16047,19 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>8.0</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D18" s="12">
         <v>139848.0</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -16096,7 +16069,7 @@
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="24" t="str">
         <f>SUM(D11:D18)</f>
@@ -16115,19 +16088,19 @@
         <v>1.0</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D20" s="12">
         <v>83591.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F20" s="14">
         <v>0.0</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H20" s="14">
         <v>48.0</v>
@@ -16141,7 +16114,7 @@
         <v>2.0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D21" s="12">
         <v>84429.0</v>
@@ -16161,7 +16134,7 @@
         <v>3.0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D22" s="12">
         <v>84874.0</v>
@@ -16181,7 +16154,7 @@
         <v>4.0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D23" s="12">
         <v>84552.0</v>
@@ -16201,13 +16174,13 @@
         <v>5.0</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D24" s="12">
         <v>134165.0</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -16227,7 +16200,7 @@
         <v>74359.0</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
@@ -16241,7 +16214,7 @@
         <v>7.0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D26" s="12">
         <v>118977.0</v>
@@ -16285,7 +16258,7 @@
       <c r="A29" s="21"/>
       <c r="B29" s="22"/>
       <c r="C29" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D29" s="24" t="str">
         <f>SUM(D20:D28)</f>
@@ -16316,7 +16289,7 @@
         <v>0.0</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H30" s="14">
         <v>59.0</v>
@@ -16336,7 +16309,7 @@
         <v>133653.0</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -16350,7 +16323,7 @@
         <v>3.0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D32" s="12">
         <v>95155.0</v>
@@ -16390,7 +16363,7 @@
         <v>5.0</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D34" s="12">
         <v>140708.0</v>
@@ -16410,7 +16383,7 @@
         <v>6.0</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D35" s="12">
         <v>160588.0</v>
@@ -16446,7 +16419,7 @@
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D38" s="34" t="str">
         <f>(D10+D19+D29+D36)</f>
@@ -19424,7 +19397,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -19466,8 +19439,8 @@
       <c r="B3" s="10">
         <v>1.0</v>
       </c>
-      <c r="C3" s="41" t="s">
-        <v>107</v>
+      <c r="C3" s="40" t="s">
+        <v>99</v>
       </c>
       <c r="D3" s="12">
         <v>101947.0</v>
@@ -19479,9 +19452,9 @@
         <v>5.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="42"/>
+        <v>100</v>
+      </c>
+      <c r="H3" s="41"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
@@ -19490,7 +19463,7 @@
       <c r="B4" s="10">
         <v>2.0</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="42" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="12">
@@ -19510,7 +19483,7 @@
       <c r="B5" s="10">
         <v>3.0</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="42" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="12">
@@ -19530,8 +19503,8 @@
       <c r="B6" s="10">
         <v>4.0</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>55</v>
+      <c r="C6" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="D6" s="12">
         <v>135435.0</v>
@@ -19550,14 +19523,14 @@
       <c r="B7" s="10">
         <v>5.0</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12">
         <v>126043.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -19570,14 +19543,14 @@
       <c r="B8" s="10">
         <v>6.0</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>71</v>
+      <c r="C8" s="43" t="s">
+        <v>63</v>
       </c>
       <c r="D8" s="20">
         <v>142559.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -19590,14 +19563,14 @@
       <c r="B9" s="10">
         <v>7.0</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>71</v>
+      <c r="C9" s="43" t="s">
+        <v>63</v>
       </c>
       <c r="D9" s="20">
         <v>141121.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -19610,14 +19583,14 @@
       <c r="B10" s="10">
         <v>8.0</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>15</v>
+      <c r="C10" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="20">
         <v>186600.0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -19630,14 +19603,14 @@
       <c r="B11" s="10">
         <v>9.0</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>15</v>
+      <c r="C11" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="20">
         <v>187071.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -19650,14 +19623,14 @@
       <c r="B12" s="10">
         <v>10.0</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>15</v>
+      <c r="C12" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D12" s="20">
         <v>186601.0</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -19667,26 +19640,26 @@
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="24" t="str">
         <f>SUM(D3:D12)</f>
         <v>1484097</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>1.0</v>
       </c>
-      <c r="C14" s="43" t="s">
-        <v>110</v>
+      <c r="C14" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="D14" s="12">
         <v>156184.0</v>
@@ -19698,25 +19671,25 @@
         <v>9.0</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="H14" s="42"/>
+        <v>103</v>
+      </c>
+      <c r="H14" s="41"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>2.0</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="43" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="12">
         <v>135125.0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -19724,19 +19697,19 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>3.0</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="12">
         <v>135766.0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -19744,19 +19717,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>4.0</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="43" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="12">
         <v>145132.0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -19764,13 +19737,13 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>5.0</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>112</v>
+      <c r="C18" s="42" t="s">
+        <v>104</v>
       </c>
       <c r="D18" s="12">
         <v>148611.0</v>
@@ -19784,19 +19757,19 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="10">
         <v>6.0</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>15</v>
+      <c r="C19" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D19" s="12">
         <v>72190.0</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
@@ -19804,19 +19777,19 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10">
         <v>7.0</v>
       </c>
-      <c r="C20" s="45" t="s">
-        <v>15</v>
+      <c r="C20" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D20" s="12">
         <v>151411.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -19826,13 +19799,13 @@
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="24" t="str">
         <f>SUM(D14:D20)</f>
         <v>944419</v>
       </c>
-      <c r="E21" s="46"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
@@ -19857,9 +19830,9 @@
         <v>7.0</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="42"/>
+        <v>105</v>
+      </c>
+      <c r="H22" s="41"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
@@ -19935,7 +19908,7 @@
         <v>136993.0</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -19968,14 +19941,14 @@
       <c r="B28" s="10">
         <v>7.0</v>
       </c>
-      <c r="C28" s="45" t="s">
-        <v>15</v>
+      <c r="C28" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="D28" s="12">
         <v>133066.0</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -20033,13 +20006,13 @@
       <c r="A32" s="21"/>
       <c r="B32" s="22"/>
       <c r="C32" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="24" t="str">
         <f>SUM(D22:D31)</f>
         <v>1084614</v>
       </c>
-      <c r="E32" s="46"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
@@ -20052,21 +20025,21 @@
         <v>1.0</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D33" s="12">
         <v>127783.0</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F33" s="14">
         <v>13.0</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H33" s="42"/>
+        <v>107</v>
+      </c>
+      <c r="H33" s="41"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
@@ -20076,13 +20049,13 @@
         <v>2.0</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D34" s="12">
         <v>145914.0</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -20096,13 +20069,13 @@
         <v>3.0</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D35" s="12">
         <v>148792.0</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -20116,7 +20089,7 @@
         <v>4.0</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D36" s="12">
         <v>148953.0</v>
@@ -20136,7 +20109,7 @@
         <v>5.0</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D37" s="12">
         <v>120022.0</v>
@@ -20156,7 +20129,7 @@
         <v>6.0</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D38" s="12">
         <v>94635.0</v>
@@ -20172,13 +20145,13 @@
       <c r="A39" s="21"/>
       <c r="B39" s="22"/>
       <c r="C39" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D39" s="24" t="str">
         <f>SUM(D33:D38)</f>
         <v>786099</v>
       </c>
-      <c r="E39" s="46"/>
+      <c r="E39" s="45"/>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
       <c r="H39" s="26"/>
@@ -20188,40 +20161,40 @@
       <c r="B40" s="8"/>
       <c r="C40" s="31"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="47"/>
+      <c r="E40" s="46"/>
     </row>
     <row r="41">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D41" s="34" t="str">
         <f>(D13+D21+D32+D39)</f>
         <v>4299229</v>
       </c>
-      <c r="E41" s="47"/>
+      <c r="E41" s="46"/>
     </row>
     <row r="42">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="31"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="47"/>
+      <c r="E42" s="46"/>
     </row>
     <row r="43">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="31"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="47"/>
+      <c r="E43" s="46"/>
     </row>
     <row r="44">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="31"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="47"/>
+      <c r="E44" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -20256,7 +20229,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -20305,15 +20278,15 @@
         <v>80501.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" s="14">
         <v>2.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="42"/>
+        <v>84</v>
+      </c>
+      <c r="H3" s="41"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
@@ -20329,7 +20302,7 @@
         <v>90796.0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -20343,13 +20316,13 @@
         <v>3.0</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D5" s="12">
         <v>198390.0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -20363,13 +20336,13 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D6" s="12">
         <v>199013.0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -20383,7 +20356,7 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D7" s="12">
         <v>183741.0</v>
@@ -20403,13 +20376,13 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="20">
         <v>193488.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -20423,13 +20396,13 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="20">
         <v>193146.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -20443,13 +20416,13 @@
         <v>8.0</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="20">
         <v>176647.0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -20463,13 +20436,13 @@
         <v>9.0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="20">
         <v>176433.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -20479,7 +20452,7 @@
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="24" t="str">
         <f>SUM(D3:D11)</f>
@@ -20492,42 +20465,42 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10">
         <v>1.0</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D13" s="12">
         <v>82615.0</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="14">
         <v>2.0</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="42"/>
+        <v>113</v>
+      </c>
+      <c r="H13" s="41"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>2.0</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D14" s="12">
         <v>196394.0</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="39" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="16"/>
@@ -20536,7 +20509,7 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>3.0</v>
@@ -20548,7 +20521,7 @@
         <v>166780.0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -20556,7 +20529,7 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>4.0</v>
@@ -20567,7 +20540,7 @@
       <c r="D16" s="12">
         <v>128522.0</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="39" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="16"/>
@@ -20576,19 +20549,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>5.0</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D17" s="12">
         <v>100000.0</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -20596,19 +20569,19 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>6.0</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D18" s="12">
         <v>199804.0</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -20618,7 +20591,7 @@
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="24" t="str">
         <f>SUM(D13:D18)</f>
@@ -20637,21 +20610,21 @@
         <v>1.0</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12">
         <v>99170.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F20" s="14">
         <v>0.0</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="42"/>
+        <v>117</v>
+      </c>
+      <c r="H20" s="41"/>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
@@ -20661,13 +20634,13 @@
         <v>2.0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D21" s="12">
         <v>99170.0</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -20687,7 +20660,7 @@
         <v>172986.0</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -20701,7 +20674,7 @@
         <v>4.0</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D23" s="12">
         <v>131066.0</v>
@@ -20721,13 +20694,13 @@
         <v>5.0</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D24" s="12">
         <v>112600.0</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -20741,7 +20714,7 @@
         <v>6.0</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D25" s="12">
         <v>191347.0</v>
@@ -20781,7 +20754,7 @@
         <v>8.0</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D27" s="12">
         <v>165100.0</v>
@@ -20797,7 +20770,7 @@
       <c r="A28" s="21"/>
       <c r="B28" s="22"/>
       <c r="C28" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" s="24" t="str">
         <f>SUM(D20:D27)</f>
@@ -20822,15 +20795,15 @@
         <v>143454.0</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F29" s="14">
         <v>0.0</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="42"/>
+        <v>64</v>
+      </c>
+      <c r="H29" s="41"/>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
@@ -20846,7 +20819,7 @@
         <v>143454.0</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -20860,13 +20833,13 @@
         <v>3.0</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D31" s="12">
         <v>121625.0</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -20880,7 +20853,7 @@
         <v>4.0</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D32" s="12">
         <v>90023.0</v>
@@ -20900,13 +20873,13 @@
         <v>5.0</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D33" s="12">
         <v>197064.0</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -20916,7 +20889,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="22"/>
       <c r="C34" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D34" s="24" t="str">
         <f>SUM(D29:D33)</f>
@@ -20938,7 +20911,7 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D36" s="34" t="str">
         <f>(D12+D19+D28+D34)</f>
@@ -23918,7 +23891,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -23950,7 +23923,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
@@ -23967,13 +23940,13 @@
         <v>161060.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" s="14">
         <v>0.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H3" s="14">
         <v>57.0</v>
@@ -23993,7 +23966,7 @@
         <v>149412.0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -24007,13 +23980,13 @@
         <v>3.0</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="20">
         <v>192733.0</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -24027,13 +24000,13 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="20">
         <v>192733.0</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -24047,13 +24020,13 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="20">
         <v>167433.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -24067,13 +24040,13 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="20">
         <v>124565.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -24087,13 +24060,13 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="20">
         <v>124431.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -24103,7 +24076,7 @@
       <c r="A10" s="21"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="24" t="str">
         <f>SUM(D3:D9)</f>
@@ -24116,25 +24089,25 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10">
         <v>1.0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D11" s="12">
         <v>179836.0</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F11" s="14">
         <v>0.0</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H11" s="14">
         <v>50.0</v>
@@ -24142,19 +24115,19 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10">
         <v>2.0</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D12" s="12">
         <v>179836.0</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -24164,7 +24137,7 @@
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="24" t="str">
         <f>SUM(D11:D12)</f>
@@ -24189,13 +24162,13 @@
         <v>171870.0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F14" s="14">
         <v>0.0</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H14" s="14">
         <v>31.0</v>
@@ -24229,7 +24202,7 @@
         <v>3.0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D16" s="12">
         <v>142192.0</v>
@@ -24259,7 +24232,7 @@
       <c r="A18" s="21"/>
       <c r="B18" s="22"/>
       <c r="C18" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="24" t="str">
         <f>SUM(D14:D17)</f>
@@ -24278,7 +24251,7 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D19" s="12">
         <v>130941.0</v>
@@ -24290,7 +24263,7 @@
         <v>0.0</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H19" s="14">
         <v>34.0</v>
@@ -24304,13 +24277,13 @@
         <v>2.0</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D20" s="12">
         <v>200000.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -24324,13 +24297,13 @@
         <v>3.0</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D21" s="12">
         <v>161437.0</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -24354,7 +24327,7 @@
       <c r="A23" s="21"/>
       <c r="B23" s="22"/>
       <c r="C23" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D23" s="24" t="str">
         <f>SUM(D19:D22)</f>
@@ -24376,7 +24349,7 @@
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D25" s="34" t="str">
         <f>(D10+D13+D18+D23)</f>
@@ -27355,7 +27328,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -27387,7 +27360,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
@@ -27398,19 +27371,19 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D3" s="12">
         <v>192004.0</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="14">
         <v>0.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H3" s="14">
         <v>93.93</v>
@@ -27424,13 +27397,13 @@
         <v>2.0</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D4" s="12">
         <v>192004.0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -27490,7 +27463,7 @@
         <v>160881.0</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -27524,13 +27497,13 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="20">
         <v>191823.0</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -27544,13 +27517,13 @@
         <v>8.0</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="20">
         <v>195882.0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -27564,13 +27537,13 @@
         <v>9.0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="20">
         <v>124561.0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -27584,13 +27557,13 @@
         <v>10.0</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="20">
         <v>146418.0</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -27600,7 +27573,7 @@
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="24" t="str">
         <f>SUM(D3:D12)</f>
@@ -27613,25 +27586,25 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
         <v>1.0</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D14" s="12">
         <v>161717.0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="14">
         <v>0.0</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H14" s="14">
         <v>98.0</v>
@@ -27639,19 +27612,19 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10">
         <v>2.0</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D15" s="12">
         <v>161717.0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -27659,19 +27632,19 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10">
         <v>3.0</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D16" s="12">
         <v>149836.0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -27679,19 +27652,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="10">
         <v>4.0</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12">
         <v>147945.0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -27699,7 +27672,7 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>5.0</v>
@@ -27719,7 +27692,7 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="10">
         <v>6.0</v>
@@ -27739,19 +27712,19 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10">
         <v>7.0</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D20" s="12">
         <v>179836.0</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -27759,19 +27732,19 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="10">
         <v>8.0</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D21" s="12">
         <v>179836.0</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -27781,7 +27754,7 @@
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="24" t="str">
         <f>SUM(D14:D21)</f>
@@ -27806,7 +27779,7 @@
         <v>172512.0</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F23" s="14">
         <v>0.0</v>
@@ -27876,7 +27849,7 @@
       <c r="A27" s="21"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="24" t="str">
         <f>SUM(D23:D26)</f>
@@ -27895,19 +27868,19 @@
         <v>1.0</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D28" s="12">
         <v>200000.0</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F28" s="14">
         <v>0.0</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H28" s="14">
         <v>94.0</v>
@@ -27915,13 +27888,13 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="48">
+        <v>38</v>
+      </c>
+      <c r="B29" s="47">
         <v>2.0</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D29" s="12">
         <v>84584.0</v>
@@ -27935,19 +27908,19 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B30" s="10">
         <v>3.0</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D30" s="12">
         <v>161382.0</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -27955,7 +27928,7 @@
     </row>
     <row r="31">
       <c r="A31" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B31" s="10">
         <v>4.0</v>
@@ -27975,19 +27948,19 @@
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B32" s="10">
         <v>5.0</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D32" s="12">
         <v>193325.0</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -27995,13 +27968,13 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B33" s="10">
         <v>6.0</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D33" s="12">
         <v>131449.0</v>
@@ -28015,19 +27988,19 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B34" s="10">
         <v>7.0</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D34" s="12">
         <v>199065.0</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -28037,7 +28010,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="22"/>
       <c r="C35" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" s="24" t="str">
         <f>SUM(D28:D34)</f>
@@ -28059,7 +28032,7 @@
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="33" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D37" s="34" t="str">
         <f>(D13+D22+D27+D35)</f>

</xml_diff>